<commit_message>
more claudia fixes and generate map button
</commit_message>
<xml_diff>
--- a/meta/geography.xlsx
+++ b/meta/geography.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reiter\Dropbox\Data Explorer 2.0\meta-to-wcde\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiareiter/Dropbox/Data Explorer 2.0/meta-to-wcde/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3F4397-DD9A-41BD-BA27-007696817437}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AEA9C7-6591-FD4D-85FA-0ADC877BC0A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28710" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iso" sheetId="1" r:id="rId1"/>
@@ -1840,48 +1840,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1897,7 +1897,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2219,14 +2219,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="K143" sqref="K143"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>421</v>
       </c>
@@ -2252,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>417</v>
       </c>
@@ -2266,7 +2268,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>417</v>
       </c>
@@ -2280,7 +2282,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>417</v>
       </c>
@@ -2294,7 +2296,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>417</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>417</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>417</v>
       </c>
@@ -2336,7 +2338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>417</v>
       </c>
@@ -2350,7 +2352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2364,7 +2366,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2378,7 +2380,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2392,7 +2394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2406,7 +2408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2420,7 +2422,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2434,7 +2436,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2448,7 +2450,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2459,7 +2461,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2470,7 +2472,7 @@
         <v>5501</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2484,7 +2486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2498,7 +2500,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2512,7 +2514,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2526,7 +2528,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2554,7 +2556,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2568,7 +2570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2582,7 +2584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2596,7 +2598,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2624,7 +2626,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2638,7 +2640,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2678,7 +2680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -2704,7 +2706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -2756,7 +2758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -2808,7 +2810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -2886,7 +2888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -2912,7 +2914,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -2938,7 +2940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2964,7 +2966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2990,7 +2992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -3016,7 +3018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -3042,7 +3044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -3068,7 +3070,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3120,7 +3122,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3146,7 +3148,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3172,7 +3174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3198,7 +3200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3224,7 +3226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3250,7 +3252,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3276,7 +3278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3302,7 +3304,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3328,7 +3330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3354,7 +3356,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -3380,7 +3382,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -3406,7 +3408,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -3432,7 +3434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -3458,7 +3460,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -3484,7 +3486,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -3510,7 +3512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -3536,7 +3538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -3562,7 +3564,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -3588,7 +3590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -3614,7 +3616,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -3640,7 +3642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -3666,7 +3668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -3692,7 +3694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -3718,7 +3720,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -3744,7 +3746,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -3770,7 +3772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -3796,7 +3798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -3822,7 +3824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -3839,7 +3841,7 @@
         <v>1</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G76" t="s">
         <v>4</v>
@@ -3848,7 +3850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -3874,7 +3876,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -3900,7 +3902,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -3926,7 +3928,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -3952,7 +3954,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -3978,7 +3980,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -4004,7 +4006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -4030,7 +4032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -4056,7 +4058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -4082,7 +4084,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -4108,7 +4110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -4134,7 +4136,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -4160,7 +4162,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -4186,7 +4188,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -4212,7 +4214,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -4238,7 +4240,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -4264,7 +4266,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -4290,7 +4292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -4316,7 +4318,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -4342,7 +4344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -4368,7 +4370,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -4394,7 +4396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -4420,7 +4422,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -4446,7 +4448,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -4472,7 +4474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -4524,7 +4526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>2</v>
       </c>
@@ -4550,7 +4552,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>2</v>
       </c>
@@ -4576,7 +4578,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>2</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -4628,7 +4630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>2</v>
       </c>
@@ -4654,7 +4656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>2</v>
       </c>
@@ -4680,7 +4682,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -4706,7 +4708,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -4758,7 +4760,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -4784,7 +4786,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -4810,7 +4812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -4836,7 +4838,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>2</v>
       </c>
@@ -4862,7 +4864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>2</v>
       </c>
@@ -4888,7 +4890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>2</v>
       </c>
@@ -4914,7 +4916,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>2</v>
       </c>
@@ -4940,7 +4942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -4966,7 +4968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>2</v>
       </c>
@@ -4992,7 +4994,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>2</v>
       </c>
@@ -5018,7 +5020,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>2</v>
       </c>
@@ -5044,7 +5046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>2</v>
       </c>
@@ -5070,7 +5072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>2</v>
       </c>
@@ -5096,7 +5098,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>2</v>
       </c>
@@ -5122,7 +5124,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>2</v>
       </c>
@@ -5148,7 +5150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>2</v>
       </c>
@@ -5174,7 +5176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>2</v>
       </c>
@@ -5200,7 +5202,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>2</v>
       </c>
@@ -5226,7 +5228,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -5252,7 +5254,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -5278,7 +5280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>2</v>
       </c>
@@ -5304,7 +5306,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>2</v>
       </c>
@@ -5330,7 +5332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -5356,7 +5358,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -5382,7 +5384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>2</v>
       </c>
@@ -5408,7 +5410,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -5434,7 +5436,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>2</v>
       </c>
@@ -5460,7 +5462,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>2</v>
       </c>
@@ -5486,7 +5488,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -5512,7 +5514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>2</v>
       </c>
@@ -5538,7 +5540,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -5555,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="F142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G142" t="s">
         <v>8</v>
@@ -5564,7 +5566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>2</v>
       </c>
@@ -5590,7 +5592,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -5616,7 +5618,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>2</v>
       </c>
@@ -5642,7 +5644,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>2</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>2</v>
       </c>
@@ -5694,7 +5696,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>2</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>2</v>
       </c>
@@ -5746,7 +5748,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -5772,7 +5774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>2</v>
       </c>
@@ -5798,7 +5800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>2</v>
       </c>
@@ -5824,7 +5826,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>2</v>
       </c>
@@ -5850,7 +5852,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>2</v>
       </c>
@@ -5876,7 +5878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -5902,7 +5904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>2</v>
       </c>
@@ -5928,7 +5930,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>2</v>
       </c>
@@ -5954,7 +5956,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>2</v>
       </c>
@@ -5980,7 +5982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>2</v>
       </c>
@@ -6006,7 +6008,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>2</v>
       </c>
@@ -6032,7 +6034,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>2</v>
       </c>
@@ -6058,7 +6060,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>2</v>
       </c>
@@ -6084,7 +6086,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>2</v>
       </c>
@@ -6110,7 +6112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -6136,7 +6138,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>2</v>
       </c>
@@ -6162,7 +6164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>2</v>
       </c>
@@ -6188,7 +6190,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>2</v>
       </c>
@@ -6214,7 +6216,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>2</v>
       </c>
@@ -6240,7 +6242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>2</v>
       </c>
@@ -6266,7 +6268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -6292,7 +6294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>2</v>
       </c>
@@ -6318,7 +6320,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>2</v>
       </c>
@@ -6344,7 +6346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>2</v>
       </c>
@@ -6370,7 +6372,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>2</v>
       </c>
@@ -6396,7 +6398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>2</v>
       </c>
@@ -6422,7 +6424,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -6448,7 +6450,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>2</v>
       </c>
@@ -6474,7 +6476,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>2</v>
       </c>
@@ -6500,7 +6502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>2</v>
       </c>
@@ -6526,7 +6528,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -6552,7 +6554,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>2</v>
       </c>
@@ -6578,7 +6580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>2</v>
       </c>
@@ -6604,7 +6606,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>2</v>
       </c>
@@ -6630,7 +6632,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -6656,7 +6658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>2</v>
       </c>
@@ -6682,7 +6684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -6708,7 +6710,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -6734,7 +6736,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -6760,7 +6762,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>2</v>
       </c>
@@ -6786,7 +6788,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -6812,7 +6814,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>2</v>
       </c>
@@ -6838,7 +6840,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>2</v>
       </c>
@@ -6864,7 +6866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>2</v>
       </c>
@@ -6890,7 +6892,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>2</v>
       </c>
@@ -6916,7 +6918,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>2</v>
       </c>
@@ -6942,7 +6944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>2</v>
       </c>
@@ -6968,7 +6970,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>2</v>
       </c>
@@ -6994,7 +6996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>2</v>
       </c>
@@ -7020,7 +7022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>2</v>
       </c>
@@ -7046,7 +7048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>2</v>
       </c>
@@ -7072,7 +7074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>2</v>
       </c>
@@ -7098,7 +7100,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>2</v>
       </c>
@@ -7124,7 +7126,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>2</v>
       </c>
@@ -7150,7 +7152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>2</v>
       </c>
@@ -7176,7 +7178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>2</v>
       </c>
@@ -7202,7 +7204,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>2</v>
       </c>
@@ -7228,7 +7230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>2</v>
       </c>
@@ -7254,7 +7256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>2</v>
       </c>
@@ -7280,7 +7282,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>2</v>
       </c>
@@ -7306,7 +7308,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>2</v>
       </c>
@@ -7332,7 +7334,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>2</v>
       </c>
@@ -7358,7 +7360,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>2</v>
       </c>
@@ -7384,7 +7386,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>2</v>
       </c>
@@ -7410,7 +7412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>2</v>
       </c>
@@ -7436,7 +7438,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>2</v>
       </c>
@@ -7462,7 +7464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>2</v>
       </c>
@@ -7488,7 +7490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>2</v>
       </c>
@@ -7514,7 +7516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>2</v>
       </c>
@@ -7540,7 +7542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>2</v>
       </c>
@@ -7566,7 +7568,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>2</v>
       </c>
@@ -7592,7 +7594,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>2</v>
       </c>
@@ -7618,7 +7620,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>2</v>
       </c>
@@ -7644,7 +7646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>2</v>
       </c>
@@ -7670,7 +7672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>2</v>
       </c>
@@ -7696,7 +7698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>2</v>
       </c>
@@ -7722,7 +7724,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>2</v>
       </c>
@@ -7748,7 +7750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>2</v>
       </c>
@@ -7774,7 +7776,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>2</v>
       </c>
@@ -7800,7 +7802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>2</v>
       </c>
@@ -7826,7 +7828,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>2</v>
       </c>
@@ -7852,7 +7854,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
tab urls and updates
</commit_message>
<xml_diff>
--- a/meta/geography.xlsx
+++ b/meta/geography.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yildiz\Dropbox\WIC Projections 2022\WCDE for Guy\meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy\Documents\GitHub\wcde-shiny\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40188363-908C-4759-85C0-4CC757F872F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8082CEF0-013D-4CA1-A8F6-E08462A7B353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="iso" sheetId="1" r:id="rId1"/>
@@ -2179,16 +2179,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>419</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>415</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>415</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>415</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>415</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>415</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>415</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>415</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2420,8 +2420,11 @@
       <c r="C16">
         <v>5500</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -2431,8 +2434,11 @@
       <c r="C17">
         <v>5501</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2446,7 +2452,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2474,7 +2480,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -2488,7 +2494,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -2502,7 +2508,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -2516,7 +2522,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -2530,7 +2536,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2544,7 +2550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -2558,7 +2564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -2586,7 +2592,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2640,7 +2646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -2692,7 +2698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -2718,7 +2724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -2744,7 +2750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -2796,7 +2802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -2848,7 +2854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -2900,7 +2906,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2926,7 +2932,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2952,7 +2958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2978,7 +2984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -3004,7 +3010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -3030,7 +3036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3056,7 +3062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3082,7 +3088,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3108,7 +3114,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3134,7 +3140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3160,7 +3166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3186,7 +3192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3264,7 +3270,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3316,7 +3322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -3342,7 +3348,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -3394,7 +3400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -3446,7 +3452,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -3472,7 +3478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -3550,7 +3556,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -3576,7 +3582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -3602,7 +3608,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -3628,7 +3634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -3680,7 +3686,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -3706,7 +3712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -3732,7 +3738,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -3758,7 +3764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -3784,7 +3790,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -3810,7 +3816,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -3888,7 +3894,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -3914,7 +3920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -3940,7 +3946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -3966,7 +3972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -3992,7 +3998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -4018,7 +4024,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -4044,7 +4050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -4070,7 +4076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -4096,7 +4102,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -4148,7 +4154,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -4200,7 +4206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -4226,7 +4232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -4252,7 +4258,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -4278,7 +4284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -4304,7 +4310,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -4330,7 +4336,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -4382,7 +4388,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -4408,7 +4414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -4434,7 +4440,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -4460,7 +4466,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -4486,7 +4492,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>2</v>
       </c>
@@ -4512,7 +4518,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>2</v>
       </c>
@@ -4538,7 +4544,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>2</v>
       </c>
@@ -4564,7 +4570,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -4590,7 +4596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>2</v>
       </c>
@@ -4616,7 +4622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>2</v>
       </c>
@@ -4642,7 +4648,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -4668,7 +4674,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -4694,7 +4700,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -4720,7 +4726,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -4746,7 +4752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -4772,7 +4778,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -4798,7 +4804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>2</v>
       </c>
@@ -4824,7 +4830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>2</v>
       </c>
@@ -4850,7 +4856,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>2</v>
       </c>
@@ -4876,7 +4882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>2</v>
       </c>
@@ -4902,7 +4908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -4928,7 +4934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>2</v>
       </c>
@@ -4954,7 +4960,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>2</v>
       </c>
@@ -4980,7 +4986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>2</v>
       </c>
@@ -5006,7 +5012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>2</v>
       </c>
@@ -5032,7 +5038,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>2</v>
       </c>
@@ -5058,7 +5064,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>2</v>
       </c>
@@ -5084,7 +5090,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>2</v>
       </c>
@@ -5110,7 +5116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>2</v>
       </c>
@@ -5136,7 +5142,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>2</v>
       </c>
@@ -5162,7 +5168,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>2</v>
       </c>
@@ -5188,7 +5194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -5214,7 +5220,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -5240,7 +5246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>2</v>
       </c>
@@ -5266,7 +5272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>2</v>
       </c>
@@ -5292,7 +5298,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -5318,7 +5324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -5344,7 +5350,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>2</v>
       </c>
@@ -5370,7 +5376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -5396,7 +5402,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>2</v>
       </c>
@@ -5422,7 +5428,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>2</v>
       </c>
@@ -5448,7 +5454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -5474,7 +5480,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>2</v>
       </c>
@@ -5500,7 +5506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -5526,7 +5532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>2</v>
       </c>
@@ -5552,7 +5558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -5578,7 +5584,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>2</v>
       </c>
@@ -5604,7 +5610,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>2</v>
       </c>
@@ -5630,7 +5636,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>2</v>
       </c>
@@ -5656,7 +5662,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>2</v>
       </c>
@@ -5682,7 +5688,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>2</v>
       </c>
@@ -5708,7 +5714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -5734,7 +5740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>2</v>
       </c>
@@ -5760,7 +5766,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>2</v>
       </c>
@@ -5786,7 +5792,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>2</v>
       </c>
@@ -5812,7 +5818,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>2</v>
       </c>
@@ -5838,7 +5844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -5864,7 +5870,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>2</v>
       </c>
@@ -5890,7 +5896,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>2</v>
       </c>
@@ -5916,7 +5922,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>2</v>
       </c>
@@ -5942,7 +5948,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>2</v>
       </c>
@@ -5968,7 +5974,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>2</v>
       </c>
@@ -5994,7 +6000,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>2</v>
       </c>
@@ -6020,7 +6026,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>2</v>
       </c>
@@ -6046,7 +6052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>2</v>
       </c>
@@ -6072,7 +6078,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -6098,7 +6104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>2</v>
       </c>
@@ -6124,7 +6130,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>2</v>
       </c>
@@ -6150,7 +6156,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>2</v>
       </c>
@@ -6176,7 +6182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>2</v>
       </c>
@@ -6202,7 +6208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>2</v>
       </c>
@@ -6228,7 +6234,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -6254,7 +6260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>2</v>
       </c>
@@ -6280,7 +6286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>2</v>
       </c>
@@ -6306,7 +6312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>2</v>
       </c>
@@ -6332,7 +6338,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>2</v>
       </c>
@@ -6358,7 +6364,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>2</v>
       </c>
@@ -6384,7 +6390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -6410,7 +6416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>2</v>
       </c>
@@ -6436,7 +6442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>2</v>
       </c>
@@ -6462,7 +6468,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>2</v>
       </c>
@@ -6488,7 +6494,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -6514,7 +6520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>2</v>
       </c>
@@ -6540,7 +6546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>2</v>
       </c>
@@ -6566,7 +6572,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>2</v>
       </c>
@@ -6592,7 +6598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -6618,7 +6624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>2</v>
       </c>
@@ -6644,7 +6650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -6670,7 +6676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -6696,7 +6702,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -6722,7 +6728,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>2</v>
       </c>
@@ -6748,7 +6754,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -6774,7 +6780,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>2</v>
       </c>
@@ -6800,7 +6806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>2</v>
       </c>
@@ -6826,7 +6832,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>2</v>
       </c>
@@ -6852,7 +6858,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>2</v>
       </c>
@@ -6878,7 +6884,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>2</v>
       </c>
@@ -6904,7 +6910,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>2</v>
       </c>
@@ -6930,7 +6936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>2</v>
       </c>
@@ -6956,7 +6962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>2</v>
       </c>
@@ -6982,7 +6988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>2</v>
       </c>
@@ -7008,7 +7014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>2</v>
       </c>
@@ -7034,7 +7040,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>2</v>
       </c>
@@ -7060,7 +7066,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>2</v>
       </c>
@@ -7086,7 +7092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>2</v>
       </c>
@@ -7112,7 +7118,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>2</v>
       </c>
@@ -7138,7 +7144,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>2</v>
       </c>
@@ -7164,7 +7170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>2</v>
       </c>
@@ -7190,7 +7196,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>2</v>
       </c>
@@ -7216,7 +7222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>2</v>
       </c>
@@ -7242,7 +7248,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>2</v>
       </c>
@@ -7268,7 +7274,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>2</v>
       </c>
@@ -7294,7 +7300,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>2</v>
       </c>
@@ -7320,7 +7326,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>2</v>
       </c>
@@ -7346,7 +7352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>2</v>
       </c>
@@ -7372,7 +7378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>2</v>
       </c>
@@ -7398,7 +7404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>2</v>
       </c>
@@ -7424,7 +7430,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>2</v>
       </c>
@@ -7450,7 +7456,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>2</v>
       </c>
@@ -7476,7 +7482,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>2</v>
       </c>
@@ -7502,7 +7508,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>2</v>
       </c>
@@ -7528,7 +7534,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>2</v>
       </c>
@@ -7554,7 +7560,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>2</v>
       </c>
@@ -7580,7 +7586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>2</v>
       </c>
@@ -7606,7 +7612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>2</v>
       </c>
@@ -7632,7 +7638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>2</v>
       </c>
@@ -7658,7 +7664,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>2</v>
       </c>
@@ -7684,7 +7690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>2</v>
       </c>
@@ -7710,7 +7716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>2</v>
       </c>
@@ -7736,7 +7742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>2</v>
       </c>
@@ -7762,7 +7768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>2</v>
       </c>
@@ -7788,7 +7794,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>2</v>
       </c>

</xml_diff>